<commit_message>
修改 cbreader2X nav 導覽目錄中重複的 B13-1.html
</commit_message>
<xml_diff>
--- a/cbreader2X/nav/simple_nav.xlsx
+++ b/cbreader2X/nav/simple_nav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cbwork\bin\cbreader2X\nav\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6AF1F0-9EFE-4D33-A16B-33BAC5FA14D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70991C6B-A693-4F1E-81F3-2073174A1D47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="21516" windowHeight="11136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simple" sheetId="1" r:id="rId1"/>
@@ -12295,9 +12295,6 @@
     <t>help/other/B/B13-1.html 釋氏六帖解題</t>
   </si>
   <si>
-    <t>help/other/B/B13-1.html 大唐西域記解題</t>
-  </si>
-  <si>
     <t>help/other/B/B14.html 編輯說明</t>
   </si>
   <si>
@@ -13482,6 +13479,10 @@
   </si>
   <si>
     <t>LC</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>help/other/B/B13-2.html 大唐西域記解題</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -14461,8 +14462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4687"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4673" workbookViewId="0">
-      <selection activeCell="D4686" sqref="D4686"/>
+    <sheetView tabSelected="1" topLeftCell="A4345" workbookViewId="0">
+      <selection activeCell="F4360" sqref="F4360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -14479,7 +14480,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>4212</v>
+        <v>4211</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -14489,7 +14490,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>4213</v>
+        <v>4212</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -14499,7 +14500,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>4214</v>
+        <v>4213</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -14509,7 +14510,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>4215</v>
+        <v>4214</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -14519,7 +14520,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>4216</v>
+        <v>4215</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -14534,7 +14535,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>4217</v>
+        <v>4216</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -14544,7 +14545,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>4218</v>
+        <v>4217</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
@@ -14564,7 +14565,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>4219</v>
+        <v>4218</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
@@ -14574,7 +14575,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>4220</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
@@ -14584,7 +14585,7 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>4221</v>
+        <v>4220</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
@@ -14599,7 +14600,7 @@
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>4222</v>
+        <v>4221</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
@@ -14609,12 +14610,12 @@
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>4223</v>
+        <v>4222</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>4224</v>
+        <v>4223</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
@@ -14624,7 +14625,7 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>4225</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
@@ -14634,7 +14635,7 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>4226</v>
+        <v>4225</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
@@ -14659,7 +14660,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>4227</v>
+        <v>4226</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
@@ -14669,7 +14670,7 @@
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>4228</v>
+        <v>4227</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
@@ -14679,17 +14680,17 @@
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>4229</v>
+        <v>4228</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>4230</v>
+        <v>4229</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>4231</v>
+        <v>4230</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
@@ -14704,12 +14705,12 @@
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>4232</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
-        <v>4233</v>
+        <v>4232</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
@@ -14724,7 +14725,7 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
-        <v>4234</v>
+        <v>4233</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
@@ -14734,7 +14735,7 @@
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>4235</v>
+        <v>4234</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
@@ -14749,7 +14750,7 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>4236</v>
+        <v>4235</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
@@ -14759,7 +14760,7 @@
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>4237</v>
+        <v>4236</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
@@ -14779,7 +14780,7 @@
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>4238</v>
+        <v>4237</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
@@ -14789,7 +14790,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
-        <v>4239</v>
+        <v>4238</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -31639,7 +31640,7 @@
     </row>
     <row r="3435" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3435" t="s">
-        <v>4471</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="3436" spans="1:5" x14ac:dyDescent="0.3">
@@ -35804,37 +35805,37 @@
     </row>
     <row r="4268" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4268" t="s">
-        <v>4240</v>
+        <v>4239</v>
       </c>
     </row>
     <row r="4269" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4269" t="s">
-        <v>4241</v>
+        <v>4240</v>
       </c>
     </row>
     <row r="4270" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4270" t="s">
-        <v>4242</v>
+        <v>4241</v>
       </c>
     </row>
     <row r="4271" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4271" t="s">
-        <v>4243</v>
+        <v>4242</v>
       </c>
     </row>
     <row r="4272" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4272" t="s">
-        <v>4244</v>
+        <v>4243</v>
       </c>
     </row>
     <row r="4273" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4273" t="s">
-        <v>4245</v>
+        <v>4244</v>
       </c>
     </row>
     <row r="4274" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4274" t="s">
-        <v>4246</v>
+        <v>4245</v>
       </c>
     </row>
     <row r="4275" spans="3:4" x14ac:dyDescent="0.3">
@@ -35849,82 +35850,82 @@
     </row>
     <row r="4277" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4277" t="s">
-        <v>4247</v>
+        <v>4246</v>
       </c>
     </row>
     <row r="4278" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4278" t="s">
-        <v>4248</v>
+        <v>4247</v>
       </c>
     </row>
     <row r="4279" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4279" t="s">
-        <v>4249</v>
+        <v>4248</v>
       </c>
     </row>
     <row r="4280" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4280" t="s">
-        <v>4250</v>
+        <v>4249</v>
       </c>
     </row>
     <row r="4281" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4281" t="s">
-        <v>4251</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="4282" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4282" t="s">
-        <v>4252</v>
+        <v>4251</v>
       </c>
     </row>
     <row r="4283" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4283" t="s">
-        <v>4253</v>
+        <v>4252</v>
       </c>
     </row>
     <row r="4284" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4284" t="s">
-        <v>4254</v>
+        <v>4253</v>
       </c>
     </row>
     <row r="4285" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4285" t="s">
-        <v>4255</v>
+        <v>4254</v>
       </c>
     </row>
     <row r="4286" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4286" t="s">
-        <v>4256</v>
+        <v>4255</v>
       </c>
     </row>
     <row r="4287" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4287" t="s">
-        <v>4257</v>
+        <v>4256</v>
       </c>
     </row>
     <row r="4288" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4288" t="s">
-        <v>4258</v>
+        <v>4257</v>
       </c>
     </row>
     <row r="4289" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4289" t="s">
-        <v>4259</v>
+        <v>4258</v>
       </c>
     </row>
     <row r="4290" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4290" t="s">
-        <v>4260</v>
+        <v>4259</v>
       </c>
     </row>
     <row r="4291" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4291" t="s">
-        <v>4261</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="4292" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4292" t="s">
-        <v>4262</v>
+        <v>4261</v>
       </c>
     </row>
     <row r="4293" spans="3:4" x14ac:dyDescent="0.3">
@@ -35939,22 +35940,22 @@
     </row>
     <row r="4295" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4295" t="s">
-        <v>4263</v>
+        <v>4262</v>
       </c>
     </row>
     <row r="4296" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4296" t="s">
-        <v>4264</v>
+        <v>4263</v>
       </c>
     </row>
     <row r="4297" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4297" t="s">
-        <v>4265</v>
+        <v>4264</v>
       </c>
     </row>
     <row r="4298" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4298" t="s">
-        <v>4266</v>
+        <v>4265</v>
       </c>
     </row>
     <row r="4299" spans="3:4" x14ac:dyDescent="0.3">
@@ -35969,92 +35970,92 @@
     </row>
     <row r="4301" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4301" t="s">
-        <v>4267</v>
+        <v>4266</v>
       </c>
     </row>
     <row r="4302" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4302" t="s">
-        <v>4268</v>
+        <v>4267</v>
       </c>
     </row>
     <row r="4303" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4303" t="s">
-        <v>4269</v>
+        <v>4268</v>
       </c>
     </row>
     <row r="4304" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4304" t="s">
-        <v>4270</v>
+        <v>4269</v>
       </c>
     </row>
     <row r="4305" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4305" t="s">
-        <v>4271</v>
+        <v>4270</v>
       </c>
     </row>
     <row r="4306" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4306" t="s">
-        <v>4272</v>
+        <v>4271</v>
       </c>
     </row>
     <row r="4307" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4307" t="s">
-        <v>4273</v>
+        <v>4272</v>
       </c>
     </row>
     <row r="4308" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4308" t="s">
-        <v>4274</v>
+        <v>4273</v>
       </c>
     </row>
     <row r="4309" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4309" t="s">
-        <v>4275</v>
+        <v>4274</v>
       </c>
     </row>
     <row r="4310" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4310" t="s">
-        <v>4276</v>
+        <v>4275</v>
       </c>
     </row>
     <row r="4311" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4311" t="s">
-        <v>4277</v>
+        <v>4276</v>
       </c>
     </row>
     <row r="4312" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4312" t="s">
-        <v>4278</v>
+        <v>4277</v>
       </c>
     </row>
     <row r="4313" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4313" t="s">
-        <v>4279</v>
+        <v>4278</v>
       </c>
     </row>
     <row r="4314" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4314" t="s">
-        <v>4280</v>
+        <v>4279</v>
       </c>
     </row>
     <row r="4315" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4315" t="s">
-        <v>4281</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="4316" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4316" t="s">
-        <v>4282</v>
+        <v>4281</v>
       </c>
     </row>
     <row r="4317" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4317" t="s">
-        <v>4283</v>
+        <v>4282</v>
       </c>
     </row>
     <row r="4318" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4318" t="s">
-        <v>4284</v>
+        <v>4283</v>
       </c>
     </row>
     <row r="4319" spans="3:4" x14ac:dyDescent="0.3">
@@ -36069,107 +36070,107 @@
     </row>
     <row r="4321" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4321" t="s">
-        <v>4285</v>
+        <v>4284</v>
       </c>
     </row>
     <row r="4322" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4322" t="s">
-        <v>4286</v>
+        <v>4285</v>
       </c>
     </row>
     <row r="4323" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4323" t="s">
-        <v>4287</v>
+        <v>4286</v>
       </c>
     </row>
     <row r="4324" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4324" t="s">
-        <v>4288</v>
+        <v>4287</v>
       </c>
     </row>
     <row r="4325" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4325" t="s">
-        <v>4289</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="4326" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4326" t="s">
-        <v>4290</v>
+        <v>4289</v>
       </c>
     </row>
     <row r="4327" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4327" t="s">
-        <v>4291</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="4328" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4328" t="s">
-        <v>4292</v>
+        <v>4291</v>
       </c>
     </row>
     <row r="4329" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4329" t="s">
-        <v>4293</v>
+        <v>4292</v>
       </c>
     </row>
     <row r="4330" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4330" t="s">
-        <v>4294</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="4331" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4331" t="s">
-        <v>4295</v>
+        <v>4294</v>
       </c>
     </row>
     <row r="4332" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4332" t="s">
-        <v>4296</v>
+        <v>4295</v>
       </c>
     </row>
     <row r="4333" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4333" t="s">
-        <v>4297</v>
+        <v>4296</v>
       </c>
     </row>
     <row r="4334" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4334" t="s">
-        <v>4298</v>
+        <v>4297</v>
       </c>
     </row>
     <row r="4335" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4335" t="s">
-        <v>4299</v>
+        <v>4298</v>
       </c>
     </row>
     <row r="4336" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4336" t="s">
-        <v>4300</v>
+        <v>4299</v>
       </c>
     </row>
     <row r="4337" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4337" t="s">
-        <v>4301</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="4338" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4338" t="s">
-        <v>4302</v>
+        <v>4301</v>
       </c>
     </row>
     <row r="4339" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4339" t="s">
-        <v>4303</v>
+        <v>4302</v>
       </c>
     </row>
     <row r="4340" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4340" t="s">
-        <v>4304</v>
+        <v>4303</v>
       </c>
     </row>
     <row r="4341" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4341" t="s">
-        <v>4305</v>
+        <v>4304</v>
       </c>
     </row>
     <row r="4342" spans="3:4" x14ac:dyDescent="0.3">
@@ -36184,42 +36185,42 @@
     </row>
     <row r="4344" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4344" t="s">
-        <v>4306</v>
+        <v>4305</v>
       </c>
     </row>
     <row r="4345" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4345" t="s">
-        <v>4307</v>
+        <v>4306</v>
       </c>
     </row>
     <row r="4346" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4346" t="s">
-        <v>4308</v>
+        <v>4307</v>
       </c>
     </row>
     <row r="4347" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4347" t="s">
-        <v>4309</v>
+        <v>4308</v>
       </c>
     </row>
     <row r="4348" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4348" t="s">
-        <v>4310</v>
+        <v>4309</v>
       </c>
     </row>
     <row r="4349" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4349" t="s">
-        <v>4311</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="4350" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4350" t="s">
-        <v>4312</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="4351" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4351" t="s">
-        <v>4313</v>
+        <v>4312</v>
       </c>
     </row>
     <row r="4352" spans="3:4" x14ac:dyDescent="0.3">
@@ -36234,12 +36235,12 @@
     </row>
     <row r="4354" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4354" t="s">
-        <v>4314</v>
+        <v>4313</v>
       </c>
     </row>
     <row r="4355" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4355" t="s">
-        <v>4315</v>
+        <v>4314</v>
       </c>
     </row>
     <row r="4356" spans="3:5" x14ac:dyDescent="0.3">
@@ -36254,17 +36255,17 @@
     </row>
     <row r="4358" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4358" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="4359" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4359" t="s">
-        <v>4091</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="4360" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4360" t="s">
-        <v>4317</v>
+        <v>4316</v>
       </c>
     </row>
     <row r="4361" spans="3:5" x14ac:dyDescent="0.3">
@@ -36274,22 +36275,22 @@
     </row>
     <row r="4362" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4362" t="s">
-        <v>4092</v>
+        <v>4091</v>
       </c>
     </row>
     <row r="4363" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4363" t="s">
-        <v>4318</v>
+        <v>4317</v>
       </c>
     </row>
     <row r="4364" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4364" t="s">
-        <v>4319</v>
+        <v>4318</v>
       </c>
     </row>
     <row r="4365" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4365" t="s">
-        <v>4093</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="4366" spans="3:5" x14ac:dyDescent="0.3">
@@ -36299,42 +36300,42 @@
     </row>
     <row r="4367" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4367" t="s">
-        <v>4320</v>
+        <v>4319</v>
       </c>
     </row>
     <row r="4368" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4368" t="s">
-        <v>4321</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="4369" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4369" t="s">
-        <v>4322</v>
+        <v>4321</v>
       </c>
     </row>
     <row r="4370" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4370" t="s">
-        <v>4323</v>
+        <v>4322</v>
       </c>
     </row>
     <row r="4371" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4371" t="s">
-        <v>4094</v>
+        <v>4093</v>
       </c>
     </row>
     <row r="4372" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4372" t="s">
-        <v>4095</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="4373" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4373" t="s">
-        <v>4096</v>
+        <v>4095</v>
       </c>
     </row>
     <row r="4374" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4374" t="s">
-        <v>4097</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="4375" spans="3:4" x14ac:dyDescent="0.3">
@@ -36344,37 +36345,37 @@
     </row>
     <row r="4376" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4376" t="s">
-        <v>4098</v>
+        <v>4097</v>
       </c>
     </row>
     <row r="4377" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4377" t="s">
-        <v>4324</v>
+        <v>4323</v>
       </c>
     </row>
     <row r="4378" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4378" t="s">
-        <v>4325</v>
+        <v>4324</v>
       </c>
     </row>
     <row r="4379" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4379" t="s">
-        <v>4326</v>
+        <v>4325</v>
       </c>
     </row>
     <row r="4380" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4380" t="s">
-        <v>4327</v>
+        <v>4326</v>
       </c>
     </row>
     <row r="4381" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4381" t="s">
-        <v>4328</v>
+        <v>4327</v>
       </c>
     </row>
     <row r="4382" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4382" t="s">
-        <v>4329</v>
+        <v>4328</v>
       </c>
     </row>
     <row r="4383" spans="3:4" x14ac:dyDescent="0.3">
@@ -36384,52 +36385,52 @@
     </row>
     <row r="4384" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4384" t="s">
-        <v>4099</v>
+        <v>4098</v>
       </c>
     </row>
     <row r="4385" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4385" t="s">
-        <v>4330</v>
+        <v>4329</v>
       </c>
     </row>
     <row r="4386" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4386" t="s">
-        <v>4331</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="4387" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4387" t="s">
-        <v>4332</v>
+        <v>4331</v>
       </c>
     </row>
     <row r="4388" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4388" t="s">
-        <v>4333</v>
+        <v>4332</v>
       </c>
     </row>
     <row r="4389" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4389" t="s">
-        <v>4334</v>
+        <v>4333</v>
       </c>
     </row>
     <row r="4390" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4390" t="s">
-        <v>4100</v>
+        <v>4099</v>
       </c>
     </row>
     <row r="4391" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4391" t="s">
-        <v>4101</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="4392" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4392" t="s">
-        <v>4335</v>
+        <v>4334</v>
       </c>
     </row>
     <row r="4393" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4393" t="s">
-        <v>4102</v>
+        <v>4101</v>
       </c>
     </row>
     <row r="4394" spans="3:5" x14ac:dyDescent="0.3">
@@ -36444,17 +36445,17 @@
     </row>
     <row r="4396" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4396" t="s">
-        <v>4103</v>
+        <v>4102</v>
       </c>
     </row>
     <row r="4397" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4397" t="s">
-        <v>4104</v>
+        <v>4103</v>
       </c>
     </row>
     <row r="4398" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4398" t="s">
-        <v>4336</v>
+        <v>4335</v>
       </c>
     </row>
     <row r="4399" spans="3:5" x14ac:dyDescent="0.3">
@@ -36464,12 +36465,12 @@
     </row>
     <row r="4400" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4400" t="s">
-        <v>4105</v>
+        <v>4104</v>
       </c>
     </row>
     <row r="4401" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4401" t="s">
-        <v>4106</v>
+        <v>4105</v>
       </c>
     </row>
     <row r="4402" spans="3:5" x14ac:dyDescent="0.3">
@@ -36479,7 +36480,7 @@
     </row>
     <row r="4403" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4403" t="s">
-        <v>4107</v>
+        <v>4106</v>
       </c>
     </row>
     <row r="4404" spans="3:5" x14ac:dyDescent="0.3">
@@ -36489,7 +36490,7 @@
     </row>
     <row r="4405" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4405" t="s">
-        <v>4108</v>
+        <v>4107</v>
       </c>
     </row>
     <row r="4406" spans="3:5" x14ac:dyDescent="0.3">
@@ -36499,7 +36500,7 @@
     </row>
     <row r="4407" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4407" t="s">
-        <v>4109</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="4408" spans="3:5" x14ac:dyDescent="0.3">
@@ -36509,7 +36510,7 @@
     </row>
     <row r="4409" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4409" t="s">
-        <v>4110</v>
+        <v>4109</v>
       </c>
     </row>
     <row r="4410" spans="3:5" x14ac:dyDescent="0.3">
@@ -36524,12 +36525,12 @@
     </row>
     <row r="4412" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4412" t="s">
-        <v>4111</v>
+        <v>4110</v>
       </c>
     </row>
     <row r="4413" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4413" t="s">
-        <v>4112</v>
+        <v>4111</v>
       </c>
     </row>
     <row r="4414" spans="3:5" x14ac:dyDescent="0.3">
@@ -36539,7 +36540,7 @@
     </row>
     <row r="4415" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4415" t="s">
-        <v>4113</v>
+        <v>4112</v>
       </c>
     </row>
     <row r="4416" spans="3:5" x14ac:dyDescent="0.3">
@@ -36549,7 +36550,7 @@
     </row>
     <row r="4417" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4417" t="s">
-        <v>4114</v>
+        <v>4113</v>
       </c>
     </row>
     <row r="4418" spans="3:5" x14ac:dyDescent="0.3">
@@ -36559,7 +36560,7 @@
     </row>
     <row r="4419" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4419" t="s">
-        <v>4115</v>
+        <v>4114</v>
       </c>
     </row>
     <row r="4420" spans="3:5" x14ac:dyDescent="0.3">
@@ -36569,7 +36570,7 @@
     </row>
     <row r="4421" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4421" t="s">
-        <v>4116</v>
+        <v>4115</v>
       </c>
     </row>
     <row r="4422" spans="3:5" x14ac:dyDescent="0.3">
@@ -36579,7 +36580,7 @@
     </row>
     <row r="4423" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4423" t="s">
-        <v>4117</v>
+        <v>4116</v>
       </c>
     </row>
     <row r="4424" spans="3:5" x14ac:dyDescent="0.3">
@@ -36589,7 +36590,7 @@
     </row>
     <row r="4425" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4425" t="s">
-        <v>4118</v>
+        <v>4117</v>
       </c>
     </row>
     <row r="4426" spans="3:5" x14ac:dyDescent="0.3">
@@ -36599,7 +36600,7 @@
     </row>
     <row r="4427" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4427" t="s">
-        <v>4337</v>
+        <v>4336</v>
       </c>
     </row>
     <row r="4428" spans="3:5" x14ac:dyDescent="0.3">
@@ -36609,22 +36610,22 @@
     </row>
     <row r="4429" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4429" t="s">
-        <v>4119</v>
+        <v>4118</v>
       </c>
     </row>
     <row r="4430" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4430" t="s">
-        <v>4338</v>
+        <v>4337</v>
       </c>
     </row>
     <row r="4431" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4431" t="s">
-        <v>4339</v>
+        <v>4338</v>
       </c>
     </row>
     <row r="4432" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4432" t="s">
-        <v>4340</v>
+        <v>4339</v>
       </c>
     </row>
     <row r="4433" spans="3:5" x14ac:dyDescent="0.3">
@@ -36634,112 +36635,112 @@
     </row>
     <row r="4434" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4434" t="s">
-        <v>4120</v>
+        <v>4119</v>
       </c>
     </row>
     <row r="4435" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4435" t="s">
-        <v>4121</v>
+        <v>4120</v>
       </c>
     </row>
     <row r="4436" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4436" t="s">
-        <v>4122</v>
+        <v>4121</v>
       </c>
     </row>
     <row r="4437" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4437" t="s">
-        <v>4123</v>
+        <v>4122</v>
       </c>
     </row>
     <row r="4438" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4438" t="s">
-        <v>4124</v>
+        <v>4123</v>
       </c>
     </row>
     <row r="4439" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4439" t="s">
-        <v>4125</v>
+        <v>4124</v>
       </c>
     </row>
     <row r="4440" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4440" t="s">
-        <v>4126</v>
+        <v>4125</v>
       </c>
     </row>
     <row r="4441" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4441" t="s">
-        <v>4127</v>
+        <v>4126</v>
       </c>
     </row>
     <row r="4442" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4442" t="s">
-        <v>4128</v>
+        <v>4127</v>
       </c>
     </row>
     <row r="4443" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4443" t="s">
-        <v>4129</v>
+        <v>4128</v>
       </c>
     </row>
     <row r="4444" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4444" t="s">
-        <v>4130</v>
+        <v>4129</v>
       </c>
     </row>
     <row r="4445" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4445" t="s">
-        <v>4131</v>
+        <v>4130</v>
       </c>
     </row>
     <row r="4446" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4446" t="s">
-        <v>4132</v>
+        <v>4131</v>
       </c>
     </row>
     <row r="4447" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4447" t="s">
-        <v>4133</v>
+        <v>4132</v>
       </c>
     </row>
     <row r="4448" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4448" t="s">
-        <v>4134</v>
+        <v>4133</v>
       </c>
     </row>
     <row r="4449" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4449" t="s">
-        <v>4135</v>
+        <v>4134</v>
       </c>
     </row>
     <row r="4450" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4450" t="s">
-        <v>4136</v>
+        <v>4135</v>
       </c>
     </row>
     <row r="4451" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4451" t="s">
-        <v>4137</v>
+        <v>4136</v>
       </c>
     </row>
     <row r="4452" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4452" t="s">
-        <v>4138</v>
+        <v>4137</v>
       </c>
     </row>
     <row r="4453" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4453" t="s">
-        <v>4139</v>
+        <v>4138</v>
       </c>
     </row>
     <row r="4454" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4454" t="s">
-        <v>4140</v>
+        <v>4139</v>
       </c>
     </row>
     <row r="4455" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4455" t="s">
-        <v>4141</v>
+        <v>4140</v>
       </c>
     </row>
     <row r="4456" spans="3:5" x14ac:dyDescent="0.3">
@@ -36759,7 +36760,7 @@
     </row>
     <row r="4459" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4459" t="s">
-        <v>4142</v>
+        <v>4141</v>
       </c>
     </row>
     <row r="4460" spans="3:5" x14ac:dyDescent="0.3">
@@ -36769,27 +36770,27 @@
     </row>
     <row r="4461" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4461" t="s">
-        <v>4143</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="4462" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4462" t="s">
-        <v>4341</v>
+        <v>4340</v>
       </c>
     </row>
     <row r="4463" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4463" t="s">
-        <v>4342</v>
+        <v>4341</v>
       </c>
     </row>
     <row r="4464" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4464" t="s">
-        <v>4343</v>
+        <v>4342</v>
       </c>
     </row>
     <row r="4465" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4465" t="s">
-        <v>4144</v>
+        <v>4143</v>
       </c>
     </row>
     <row r="4466" spans="3:5" x14ac:dyDescent="0.3">
@@ -36799,52 +36800,52 @@
     </row>
     <row r="4467" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4467" t="s">
-        <v>4145</v>
+        <v>4144</v>
       </c>
     </row>
     <row r="4468" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4468" t="s">
-        <v>4146</v>
+        <v>4145</v>
       </c>
     </row>
     <row r="4469" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4469" t="s">
-        <v>4344</v>
+        <v>4343</v>
       </c>
     </row>
     <row r="4470" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4470" t="s">
-        <v>4345</v>
+        <v>4344</v>
       </c>
     </row>
     <row r="4471" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4471" t="s">
-        <v>4346</v>
+        <v>4345</v>
       </c>
     </row>
     <row r="4472" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4472" t="s">
-        <v>4147</v>
+        <v>4146</v>
       </c>
     </row>
     <row r="4473" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4473" t="s">
-        <v>4347</v>
+        <v>4346</v>
       </c>
     </row>
     <row r="4474" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4474" t="s">
-        <v>4348</v>
+        <v>4347</v>
       </c>
     </row>
     <row r="4475" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4475" t="s">
-        <v>4349</v>
+        <v>4348</v>
       </c>
     </row>
     <row r="4476" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4476" t="s">
-        <v>4350</v>
+        <v>4349</v>
       </c>
     </row>
     <row r="4477" spans="3:5" x14ac:dyDescent="0.3">
@@ -36854,27 +36855,27 @@
     </row>
     <row r="4478" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4478" t="s">
-        <v>4148</v>
+        <v>4147</v>
       </c>
     </row>
     <row r="4479" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4479" t="s">
-        <v>4351</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="4480" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4480" t="s">
-        <v>4352</v>
+        <v>4351</v>
       </c>
     </row>
     <row r="4481" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4481" t="s">
-        <v>4353</v>
+        <v>4352</v>
       </c>
     </row>
     <row r="4482" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4482" t="s">
-        <v>4354</v>
+        <v>4353</v>
       </c>
     </row>
     <row r="4483" spans="3:5" x14ac:dyDescent="0.3">
@@ -36884,32 +36885,32 @@
     </row>
     <row r="4484" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4484" t="s">
-        <v>4149</v>
+        <v>4148</v>
       </c>
     </row>
     <row r="4485" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4485" t="s">
-        <v>4355</v>
+        <v>4354</v>
       </c>
     </row>
     <row r="4486" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4486" t="s">
-        <v>4356</v>
+        <v>4355</v>
       </c>
     </row>
     <row r="4487" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4487" t="s">
-        <v>4357</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="4488" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4488" t="s">
-        <v>4358</v>
+        <v>4357</v>
       </c>
     </row>
     <row r="4489" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4489" t="s">
-        <v>4150</v>
+        <v>4149</v>
       </c>
     </row>
     <row r="4490" spans="3:5" x14ac:dyDescent="0.3">
@@ -36919,7 +36920,7 @@
     </row>
     <row r="4491" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4491" t="s">
-        <v>4151</v>
+        <v>4150</v>
       </c>
     </row>
     <row r="4492" spans="3:5" x14ac:dyDescent="0.3">
@@ -36929,22 +36930,22 @@
     </row>
     <row r="4493" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4493" t="s">
-        <v>4152</v>
+        <v>4151</v>
       </c>
     </row>
     <row r="4494" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4494" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
     </row>
     <row r="4495" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4495" t="s">
-        <v>4360</v>
+        <v>4359</v>
       </c>
     </row>
     <row r="4496" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4496" t="s">
-        <v>4361</v>
+        <v>4360</v>
       </c>
     </row>
     <row r="4497" spans="3:5" x14ac:dyDescent="0.3">
@@ -36954,12 +36955,12 @@
     </row>
     <row r="4498" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4498" t="s">
-        <v>4153</v>
+        <v>4152</v>
       </c>
     </row>
     <row r="4499" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4499" t="s">
-        <v>4154</v>
+        <v>4153</v>
       </c>
     </row>
     <row r="4500" spans="3:5" x14ac:dyDescent="0.3">
@@ -36969,27 +36970,27 @@
     </row>
     <row r="4501" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4501" t="s">
-        <v>4362</v>
+        <v>4361</v>
       </c>
     </row>
     <row r="4502" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4502" t="s">
-        <v>4363</v>
+        <v>4362</v>
       </c>
     </row>
     <row r="4503" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4503" t="s">
-        <v>4364</v>
+        <v>4363</v>
       </c>
     </row>
     <row r="4504" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4504" t="s">
-        <v>4365</v>
+        <v>4364</v>
       </c>
     </row>
     <row r="4505" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4505" t="s">
-        <v>4366</v>
+        <v>4365</v>
       </c>
     </row>
     <row r="4506" spans="3:5" x14ac:dyDescent="0.3">
@@ -36999,27 +37000,27 @@
     </row>
     <row r="4507" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4507" t="s">
-        <v>4155</v>
+        <v>4154</v>
       </c>
     </row>
     <row r="4508" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4508" t="s">
-        <v>4367</v>
+        <v>4366</v>
       </c>
     </row>
     <row r="4509" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4509" t="s">
-        <v>4368</v>
+        <v>4367</v>
       </c>
     </row>
     <row r="4510" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4510" t="s">
-        <v>4156</v>
+        <v>4155</v>
       </c>
     </row>
     <row r="4511" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4511" t="s">
-        <v>4157</v>
+        <v>4156</v>
       </c>
     </row>
     <row r="4512" spans="3:5" x14ac:dyDescent="0.3">
@@ -37029,62 +37030,62 @@
     </row>
     <row r="4513" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4513" t="s">
-        <v>4158</v>
+        <v>4157</v>
       </c>
     </row>
     <row r="4514" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4514" t="s">
-        <v>4369</v>
+        <v>4368</v>
       </c>
     </row>
     <row r="4515" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4515" t="s">
-        <v>4159</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="4516" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4516" t="s">
-        <v>4160</v>
+        <v>4159</v>
       </c>
     </row>
     <row r="4517" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4517" t="s">
-        <v>4161</v>
+        <v>4160</v>
       </c>
     </row>
     <row r="4518" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4518" t="s">
-        <v>4162</v>
+        <v>4161</v>
       </c>
     </row>
     <row r="4519" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4519" t="s">
-        <v>4163</v>
+        <v>4162</v>
       </c>
     </row>
     <row r="4520" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4520" t="s">
-        <v>4164</v>
+        <v>4163</v>
       </c>
     </row>
     <row r="4521" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4521" t="s">
-        <v>4165</v>
+        <v>4164</v>
       </c>
     </row>
     <row r="4522" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4522" t="s">
-        <v>4166</v>
+        <v>4165</v>
       </c>
     </row>
     <row r="4523" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4523" t="s">
-        <v>4167</v>
+        <v>4166</v>
       </c>
     </row>
     <row r="4524" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4524" t="s">
-        <v>4168</v>
+        <v>4167</v>
       </c>
     </row>
     <row r="4525" spans="3:5" x14ac:dyDescent="0.3">
@@ -37094,17 +37095,17 @@
     </row>
     <row r="4526" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4526" t="s">
-        <v>4169</v>
+        <v>4168</v>
       </c>
     </row>
     <row r="4527" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4527" t="s">
-        <v>4370</v>
+        <v>4369</v>
       </c>
     </row>
     <row r="4528" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4528" t="s">
-        <v>4371</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="4529" spans="3:4" x14ac:dyDescent="0.3">
@@ -37114,117 +37115,117 @@
     </row>
     <row r="4530" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4530" t="s">
-        <v>4170</v>
+        <v>4169</v>
       </c>
     </row>
     <row r="4531" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4531" t="s">
-        <v>4372</v>
+        <v>4371</v>
       </c>
     </row>
     <row r="4532" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4532" t="s">
-        <v>4373</v>
+        <v>4372</v>
       </c>
     </row>
     <row r="4533" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4533" t="s">
-        <v>4374</v>
+        <v>4373</v>
       </c>
     </row>
     <row r="4534" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4534" t="s">
-        <v>4375</v>
+        <v>4374</v>
       </c>
     </row>
     <row r="4535" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4535" t="s">
-        <v>4376</v>
+        <v>4375</v>
       </c>
     </row>
     <row r="4536" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4536" t="s">
-        <v>4377</v>
+        <v>4376</v>
       </c>
     </row>
     <row r="4537" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4537" t="s">
-        <v>4378</v>
+        <v>4377</v>
       </c>
     </row>
     <row r="4538" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4538" t="s">
-        <v>4379</v>
+        <v>4378</v>
       </c>
     </row>
     <row r="4539" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4539" t="s">
-        <v>4380</v>
+        <v>4379</v>
       </c>
     </row>
     <row r="4540" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4540" t="s">
-        <v>4381</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="4541" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4541" t="s">
-        <v>4382</v>
+        <v>4381</v>
       </c>
     </row>
     <row r="4542" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4542" t="s">
-        <v>4383</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="4543" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4543" t="s">
-        <v>4384</v>
+        <v>4383</v>
       </c>
     </row>
     <row r="4544" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4544" t="s">
-        <v>4385</v>
+        <v>4384</v>
       </c>
     </row>
     <row r="4545" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4545" t="s">
-        <v>4386</v>
+        <v>4385</v>
       </c>
     </row>
     <row r="4546" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4546" t="s">
-        <v>4387</v>
+        <v>4386</v>
       </c>
     </row>
     <row r="4547" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4547" t="s">
-        <v>4388</v>
+        <v>4387</v>
       </c>
     </row>
     <row r="4548" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4548" t="s">
-        <v>4171</v>
+        <v>4170</v>
       </c>
     </row>
     <row r="4549" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E4549" t="s">
-        <v>4172</v>
+        <v>4171</v>
       </c>
     </row>
     <row r="4550" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4550" t="s">
-        <v>4389</v>
+        <v>4388</v>
       </c>
     </row>
     <row r="4551" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4551" t="s">
-        <v>4390</v>
+        <v>4389</v>
       </c>
     </row>
     <row r="4552" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4552" t="s">
-        <v>4391</v>
+        <v>4390</v>
       </c>
     </row>
     <row r="4553" spans="3:5" x14ac:dyDescent="0.3">
@@ -37234,12 +37235,12 @@
     </row>
     <row r="4554" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4554" t="s">
-        <v>4173</v>
+        <v>4172</v>
       </c>
     </row>
     <row r="4555" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4555" t="s">
-        <v>4392</v>
+        <v>4391</v>
       </c>
     </row>
     <row r="4556" spans="3:5" x14ac:dyDescent="0.3">
@@ -37249,17 +37250,17 @@
     </row>
     <row r="4557" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4557" t="s">
-        <v>4174</v>
+        <v>4173</v>
       </c>
     </row>
     <row r="4558" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4558" t="s">
-        <v>4175</v>
+        <v>4174</v>
       </c>
     </row>
     <row r="4559" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4559" t="s">
-        <v>4393</v>
+        <v>4392</v>
       </c>
     </row>
     <row r="4560" spans="3:5" x14ac:dyDescent="0.3">
@@ -37269,22 +37270,22 @@
     </row>
     <row r="4561" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4561" t="s">
-        <v>4176</v>
+        <v>4175</v>
       </c>
     </row>
     <row r="4562" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4562" t="s">
-        <v>4394</v>
+        <v>4393</v>
       </c>
     </row>
     <row r="4563" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4563" t="s">
-        <v>4395</v>
+        <v>4394</v>
       </c>
     </row>
     <row r="4564" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4564" t="s">
-        <v>4396</v>
+        <v>4395</v>
       </c>
     </row>
     <row r="4565" spans="2:4" x14ac:dyDescent="0.3">
@@ -37294,612 +37295,612 @@
     </row>
     <row r="4566" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4566" t="s">
-        <v>4177</v>
+        <v>4176</v>
       </c>
     </row>
     <row r="4567" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4567" t="s">
-        <v>4397</v>
+        <v>4396</v>
       </c>
     </row>
     <row r="4568" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4568" t="s">
-        <v>4398</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="4569" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4569" t="s">
-        <v>4178</v>
+        <v>4177</v>
       </c>
     </row>
     <row r="4570" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4570" t="s">
-        <v>4179</v>
+        <v>4178</v>
       </c>
     </row>
     <row r="4571" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4571" t="s">
-        <v>4180</v>
+        <v>4179</v>
       </c>
     </row>
     <row r="4572" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4572" t="s">
-        <v>4181</v>
+        <v>4180</v>
       </c>
     </row>
     <row r="4573" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4573" t="s">
-        <v>4399</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="4574" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4574" t="s">
-        <v>4182</v>
+        <v>4181</v>
       </c>
     </row>
     <row r="4575" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4575" t="s">
-        <v>4400</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="4576" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4576" t="s">
-        <v>4183</v>
+        <v>4182</v>
       </c>
     </row>
     <row r="4577" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4577" t="s">
-        <v>4401</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="4578" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4578" t="s">
-        <v>4184</v>
+        <v>4183</v>
       </c>
     </row>
     <row r="4579" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4579" t="s">
-        <v>4402</v>
+        <v>4401</v>
       </c>
     </row>
     <row r="4580" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4580" t="s">
-        <v>4185</v>
+        <v>4184</v>
       </c>
     </row>
     <row r="4581" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4581" t="s">
-        <v>4403</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="4582" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4582" t="s">
-        <v>4186</v>
+        <v>4185</v>
       </c>
     </row>
     <row r="4583" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4583" t="s">
-        <v>4404</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="4584" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4584" t="s">
-        <v>4187</v>
+        <v>4186</v>
       </c>
     </row>
     <row r="4585" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4585" t="s">
-        <v>4188</v>
+        <v>4187</v>
       </c>
     </row>
     <row r="4586" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4586" t="s">
-        <v>4189</v>
+        <v>4188</v>
       </c>
     </row>
     <row r="4587" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4587" t="s">
-        <v>4405</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="4588" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4588" t="s">
-        <v>4190</v>
+        <v>4189</v>
       </c>
     </row>
     <row r="4589" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4589" t="s">
-        <v>4191</v>
+        <v>4190</v>
       </c>
     </row>
     <row r="4590" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4590" t="s">
-        <v>4192</v>
+        <v>4191</v>
       </c>
     </row>
     <row r="4591" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4591" t="s">
-        <v>4406</v>
+        <v>4405</v>
       </c>
     </row>
     <row r="4592" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4592" t="s">
-        <v>4193</v>
+        <v>4192</v>
       </c>
     </row>
     <row r="4593" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4593" t="s">
-        <v>4407</v>
+        <v>4406</v>
       </c>
     </row>
     <row r="4594" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4594" t="s">
-        <v>4194</v>
+        <v>4193</v>
       </c>
     </row>
     <row r="4595" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4595" t="s">
-        <v>4408</v>
+        <v>4407</v>
       </c>
     </row>
     <row r="4596" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4596" t="s">
-        <v>4195</v>
+        <v>4194</v>
       </c>
     </row>
     <row r="4597" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4597" t="s">
-        <v>4409</v>
+        <v>4408</v>
       </c>
     </row>
     <row r="4598" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4598" t="s">
-        <v>4410</v>
+        <v>4409</v>
       </c>
     </row>
     <row r="4599" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4599" t="s">
-        <v>4411</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="4600" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4600" t="s">
-        <v>4412</v>
+        <v>4411</v>
       </c>
     </row>
     <row r="4601" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4601" t="s">
-        <v>4413</v>
+        <v>4412</v>
       </c>
     </row>
     <row r="4602" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4602" t="s">
-        <v>4414</v>
+        <v>4413</v>
       </c>
     </row>
     <row r="4603" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4603" t="s">
-        <v>4415</v>
+        <v>4414</v>
       </c>
     </row>
     <row r="4604" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4604" t="s">
-        <v>4416</v>
+        <v>4415</v>
       </c>
     </row>
     <row r="4605" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4605" t="s">
-        <v>4417</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="4606" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4606" t="s">
-        <v>4418</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="4607" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4607" t="s">
-        <v>4419</v>
+        <v>4418</v>
       </c>
     </row>
     <row r="4608" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4608" t="s">
-        <v>4420</v>
+        <v>4419</v>
       </c>
     </row>
     <row r="4609" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4609" t="s">
-        <v>4421</v>
+        <v>4420</v>
       </c>
     </row>
     <row r="4610" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4610" t="s">
-        <v>4196</v>
+        <v>4195</v>
       </c>
     </row>
     <row r="4611" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4611" t="s">
-        <v>4197</v>
+        <v>4196</v>
       </c>
     </row>
     <row r="4612" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4612" t="s">
-        <v>4422</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="4613" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4613" t="s">
-        <v>4198</v>
+        <v>4197</v>
       </c>
     </row>
     <row r="4614" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4614" t="s">
-        <v>4423</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="4615" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4615" t="s">
-        <v>4199</v>
+        <v>4198</v>
       </c>
     </row>
     <row r="4616" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4616" t="s">
-        <v>4424</v>
+        <v>4423</v>
       </c>
     </row>
     <row r="4617" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4617" t="s">
-        <v>4425</v>
+        <v>4424</v>
       </c>
     </row>
     <row r="4618" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4618" t="s">
-        <v>4426</v>
+        <v>4425</v>
       </c>
     </row>
     <row r="4619" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4619" t="s">
-        <v>4427</v>
+        <v>4426</v>
       </c>
     </row>
     <row r="4620" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4620" t="s">
-        <v>4200</v>
+        <v>4199</v>
       </c>
     </row>
     <row r="4621" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4621" t="s">
-        <v>4428</v>
+        <v>4427</v>
       </c>
     </row>
     <row r="4622" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4622" t="s">
-        <v>4201</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="4623" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4623" t="s">
-        <v>4202</v>
+        <v>4201</v>
       </c>
     </row>
     <row r="4624" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4624" t="s">
-        <v>4203</v>
+        <v>4202</v>
       </c>
     </row>
     <row r="4625" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D4625" t="s">
-        <v>4475</v>
+        <v>4474</v>
       </c>
     </row>
     <row r="4626" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4626" t="s">
-        <v>4476</v>
+        <v>4475</v>
       </c>
     </row>
     <row r="4627" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C4627" t="s">
-        <v>4204</v>
+        <v>4203</v>
       </c>
     </row>
     <row r="4628" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D4628" t="s">
-        <v>4472</v>
+        <v>4471</v>
       </c>
     </row>
     <row r="4629" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4629" t="s">
-        <v>4429</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="4630" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4630" t="s">
-        <v>4430</v>
+        <v>4429</v>
       </c>
     </row>
     <row r="4631" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4631" t="s">
-        <v>4431</v>
+        <v>4430</v>
       </c>
     </row>
     <row r="4632" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4632" t="s">
-        <v>4432</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="4633" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4633" t="s">
-        <v>4433</v>
+        <v>4432</v>
       </c>
     </row>
     <row r="4634" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4634" t="s">
-        <v>4434</v>
+        <v>4433</v>
       </c>
     </row>
     <row r="4635" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4635" t="s">
-        <v>4435</v>
+        <v>4434</v>
       </c>
     </row>
     <row r="4636" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D4636" t="s">
-        <v>4473</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="4637" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4637" t="s">
-        <v>4436</v>
+        <v>4435</v>
       </c>
     </row>
     <row r="4638" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4638" t="s">
-        <v>4437</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="4639" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4639" t="s">
-        <v>4438</v>
+        <v>4437</v>
       </c>
     </row>
     <row r="4640" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4640" t="s">
-        <v>4439</v>
+        <v>4438</v>
       </c>
     </row>
     <row r="4641" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4641" t="s">
-        <v>4440</v>
+        <v>4439</v>
       </c>
     </row>
     <row r="4642" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4642" t="s">
-        <v>4441</v>
+        <v>4440</v>
       </c>
     </row>
     <row r="4643" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4643" t="s">
-        <v>4442</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="4644" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D4644" t="s">
-        <v>4474</v>
+        <v>4473</v>
       </c>
     </row>
     <row r="4645" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4645" t="s">
-        <v>4443</v>
+        <v>4442</v>
       </c>
     </row>
     <row r="4646" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4646" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="4647" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4647" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="4648" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4648" t="s">
-        <v>4446</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="4649" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4649" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="4650" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4650" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="4651" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4651" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="4652" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4652" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="4653" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4653" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="4654" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4654" t="s">
-        <v>4452</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="4655" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4655" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="4656" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E4656" t="s">
-        <v>4454</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="4657" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4657" t="s">
-        <v>4205</v>
+        <v>4204</v>
       </c>
     </row>
     <row r="4658" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4658" t="s">
-        <v>4455</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="4659" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4659" t="s">
-        <v>4456</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="4660" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4660" t="s">
-        <v>4457</v>
+        <v>4456</v>
       </c>
     </row>
     <row r="4661" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4661" t="s">
-        <v>4458</v>
+        <v>4457</v>
       </c>
     </row>
     <row r="4662" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4662" t="s">
-        <v>4459</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="4663" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4663" t="s">
-        <v>4206</v>
+        <v>4205</v>
       </c>
     </row>
     <row r="4664" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4664" t="s">
-        <v>4460</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="4665" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4665" t="s">
-        <v>4461</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="4666" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4666" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="4667" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4667" t="s">
-        <v>4463</v>
+        <v>4462</v>
       </c>
     </row>
     <row r="4668" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4668" t="s">
-        <v>4464</v>
+        <v>4463</v>
       </c>
     </row>
     <row r="4669" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4669" t="s">
-        <v>4465</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="4670" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4670" t="s">
-        <v>4477</v>
+        <v>4476</v>
       </c>
     </row>
     <row r="4671" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4671" t="s">
-        <v>4478</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="4672" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D4672" t="s">
-        <v>4466</v>
+        <v>4465</v>
       </c>
     </row>
     <row r="4673" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4673" t="s">
-        <v>4479</v>
+        <v>4478</v>
       </c>
     </row>
     <row r="4674" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4674" t="s">
-        <v>4480</v>
+        <v>4479</v>
       </c>
     </row>
     <row r="4675" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4675" t="s">
-        <v>4467</v>
+        <v>4466</v>
       </c>
     </row>
     <row r="4676" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4676" t="s">
-        <v>4481</v>
+        <v>4480</v>
       </c>
     </row>
     <row r="4677" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4677" t="s">
-        <v>4482</v>
+        <v>4481</v>
       </c>
     </row>
     <row r="4678" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4678" t="s">
-        <v>4468</v>
+        <v>4467</v>
       </c>
     </row>
     <row r="4679" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4679" t="s">
-        <v>4469</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="4680" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4680" t="s">
-        <v>4470</v>
+        <v>4469</v>
       </c>
     </row>
     <row r="4681" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4681" t="s">
-        <v>4207</v>
+        <v>4206</v>
       </c>
     </row>
     <row r="4682" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4682" t="s">
-        <v>4208</v>
+        <v>4207</v>
       </c>
     </row>
     <row r="4683" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4683" t="s">
-        <v>4209</v>
+        <v>4208</v>
       </c>
     </row>
     <row r="4684" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4684" t="s">
-        <v>4210</v>
+        <v>4209</v>
       </c>
     </row>
     <row r="4685" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D4685" t="s">
-        <v>4211</v>
+        <v>4210</v>
       </c>
     </row>
     <row r="4686" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4686" t="s">
-        <v>4483</v>
+        <v>4482</v>
       </c>
     </row>
     <row r="4687" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4687" t="s">
-        <v>4484</v>
+        <v>4483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>